<commit_message>
Menu avec test de rotation
J'ai enfin commencer à utiliser Kotlin, pas facile apprendre rapidement un nouveau langage, mais toujours un défi aggréable.
Les tests de rotation sont concluant, mais sa semble pas être le top sur mon téléphone comparer à l'émulateur, une correction s'impose
</commit_message>
<xml_diff>
--- a/Doc/estimation.xlsx
+++ b/Doc/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -119,10 +119,40 @@
     <t>* Les période du mardi matin sont obligatoires. Les autres seront réservés aux questions et rencontres</t>
   </si>
   <si>
-    <t>Exploration et apprentissage du Canvas</t>
-  </si>
-  <si>
     <t>10h</t>
+  </si>
+  <si>
+    <t>Animation sur Canvas</t>
+  </si>
+  <si>
+    <t>Création et changement d'aactivité pour arrivé dans les menus</t>
+  </si>
+  <si>
+    <t>charger les données dans la BD SQLite</t>
+  </si>
+  <si>
+    <t>2 heures</t>
+  </si>
+  <si>
+    <t>1 heure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup du git et partage avec l'enseignant </t>
+  </si>
+  <si>
+    <t>Apprentissage du Canvas pour les animations</t>
+  </si>
+  <si>
+    <t>mise en pratique par rotation d'une image</t>
+  </si>
+  <si>
+    <t>2 heure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apprentissage du Kotlin et des méthode d'animations intégré </t>
+  </si>
+  <si>
+    <t>3 heures</t>
   </si>
 </sst>
 </file>
@@ -266,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,6 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1574,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,24 +1663,28 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1786,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,24 +1879,48 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>43178</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="23">
+        <v>43179</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="23">
+        <v>43180</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="23">
+        <v>43180</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>

</xml_diff>